<commit_message>
Cambios en el documento y las plantillas para la versión 3
</commit_message>
<xml_diff>
--- a/Procesos/ControlDeCambios/DP_Plantillas_ControldeCambios_Grupo2.xlsx
+++ b/Procesos/ControlDeCambios/DP_Plantillas_ControldeCambios_Grupo2.xlsx
@@ -5,15 +5,15 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nubeusc-my.sharepoint.com/personal/guillermo_arcos_rai_usc_es/Documents/Practica6_gestionconfiguracion/Entrega 1/v2/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://nubeusc-my.sharepoint.com/personal/guillermo_arcos_rai_usc_es/Documents/Practica6_gestionconfiguracion/Entrega 2/v3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="724" documentId="11_3E5E55BF84DCCE83696592588431F45B0A7454DF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{37F1C372-B7CE-4EFA-ABDE-8AFCAFB2196D}"/>
+  <xr:revisionPtr revIDLastSave="880" documentId="11_3E5E55BF84DCCE83696592588431F45B0A7454DF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FC690589-7B62-4288-8622-EAF321104AB8}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1176" windowWidth="23040" windowHeight="11016" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Identificación del problema" sheetId="1" r:id="rId1"/>
+    <sheet name="Identificación del problema" sheetId="10" r:id="rId1"/>
     <sheet name="Informe del cambio" sheetId="2" r:id="rId2"/>
     <sheet name="Aprobación del cambio" sheetId="3" r:id="rId3"/>
     <sheet name="ECO" sheetId="4" r:id="rId4"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="58">
   <si>
     <t>IdP:</t>
   </si>
@@ -190,13 +190,52 @@
   </si>
   <si>
     <t>Fecha de notificación:</t>
+  </si>
+  <si>
+    <t>Coste Temporal (Scrum Poker)</t>
+  </si>
+  <si>
+    <t>Votación 1</t>
+  </si>
+  <si>
+    <t>Votación 2</t>
+  </si>
+  <si>
+    <t>Votación 3</t>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>M</t>
+    </r>
+  </si>
+  <si>
+    <t>M1</t>
+  </si>
+  <si>
+    <t>M2</t>
+  </si>
+  <si>
+    <t>M3</t>
+  </si>
+  <si>
+    <t>M4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,8 +279,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -254,8 +307,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="23">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -497,11 +556,37 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -522,13 +607,64 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -537,16 +673,25 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -621,6 +766,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -639,6 +787,57 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -648,33 +847,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -719,15 +891,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -824,6 +987,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
+      <color rgb="FFEEEEEE"/>
       <color rgb="FFFF7C80"/>
       <color rgb="FFA50021"/>
       <color rgb="FFFF5050"/>
@@ -1161,180 +1325,180 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26FD3CFE-7DC5-45B5-A96F-74D961D3ED11}">
   <dimension ref="B2:I14"/>
   <sheetViews>
     <sheetView zoomScale="77" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I14"/>
+      <selection activeCell="L17" sqref="L17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="20.25" customHeight="1" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="27"/>
     </row>
     <row r="3" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13" t="s">
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="32"/>
     </row>
     <row r="4" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="16"/>
-      <c r="F4" s="11" t="s">
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
+      <c r="E4" s="33"/>
+      <c r="F4" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="12"/>
-      <c r="H4" s="12"/>
-      <c r="I4" s="16"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="36"/>
     </row>
     <row r="5" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="26" t="s">
+      <c r="B5" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="28"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="47"/>
+      <c r="G5" s="47"/>
+      <c r="H5" s="47"/>
+      <c r="I5" s="48"/>
     </row>
     <row r="6" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="49" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="30"/>
-      <c r="H6" s="30"/>
-      <c r="I6" s="31"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+      <c r="H6" s="50"/>
+      <c r="I6" s="51"/>
     </row>
     <row r="7" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="32"/>
-      <c r="C7" s="33"/>
-      <c r="D7" s="33"/>
-      <c r="E7" s="33"/>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="33"/>
-      <c r="I7" s="34"/>
+      <c r="B7" s="52"/>
+      <c r="C7" s="53"/>
+      <c r="D7" s="53"/>
+      <c r="E7" s="53"/>
+      <c r="F7" s="53"/>
+      <c r="G7" s="53"/>
+      <c r="H7" s="53"/>
+      <c r="I7" s="54"/>
     </row>
     <row r="8" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="55" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="36"/>
-      <c r="D8" s="36"/>
-      <c r="E8" s="36"/>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36"/>
-      <c r="H8" s="36"/>
-      <c r="I8" s="37"/>
+      <c r="C8" s="56"/>
+      <c r="D8" s="56"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="56"/>
+      <c r="G8" s="56"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="57"/>
     </row>
     <row r="9" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="38"/>
-      <c r="C9" s="39"/>
-      <c r="D9" s="39"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="39"/>
-      <c r="H9" s="39"/>
-      <c r="I9" s="40"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="59"/>
+      <c r="F9" s="59"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="60"/>
     </row>
     <row r="10" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="49" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="30"/>
-      <c r="D10" s="30"/>
-      <c r="E10" s="30"/>
-      <c r="F10" s="30"/>
-      <c r="G10" s="30"/>
-      <c r="H10" s="30"/>
-      <c r="I10" s="31"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+      <c r="H10" s="50"/>
+      <c r="I10" s="51"/>
     </row>
     <row r="11" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="32"/>
-      <c r="C11" s="33"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="34"/>
+      <c r="B11" s="52"/>
+      <c r="C11" s="53"/>
+      <c r="D11" s="53"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+      <c r="H11" s="53"/>
+      <c r="I11" s="54"/>
     </row>
     <row r="12" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="18"/>
-      <c r="D12" s="18"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="18"/>
-      <c r="I12" s="19"/>
+      <c r="C12" s="38"/>
+      <c r="D12" s="38"/>
+      <c r="E12" s="38"/>
+      <c r="F12" s="38"/>
+      <c r="G12" s="38"/>
+      <c r="H12" s="38"/>
+      <c r="I12" s="39"/>
     </row>
     <row r="13" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="22"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="42"/>
     </row>
     <row r="14" spans="2:9" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="24"/>
-      <c r="F14" s="24"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="25"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="44"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="44"/>
+      <c r="G14" s="44"/>
+      <c r="H14" s="44"/>
+      <c r="I14" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="B12:I12"/>
-    <mergeCell ref="B13:I13"/>
     <mergeCell ref="B14:I14"/>
     <mergeCell ref="B5:I5"/>
     <mergeCell ref="B6:I7"/>
     <mergeCell ref="B8:I9"/>
     <mergeCell ref="B10:I11"/>
+    <mergeCell ref="B12:I12"/>
+    <mergeCell ref="B13:I13"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="B3:E3"/>
@@ -1343,35 +1507,40 @@
     <mergeCell ref="F4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBE3CBD3-8E5F-4950-99AB-534644994998}">
-  <dimension ref="B2:I22"/>
+  <dimension ref="B2:I28"/>
   <sheetViews>
-    <sheetView zoomScale="103" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:I18"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.6640625"/>
+    <col min="2" max="2" width="2.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.6640625" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" customWidth="1"/>
+    <col min="8" max="8" width="13.88671875" customWidth="1"/>
+    <col min="9" max="9" width="3.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
@@ -1386,184 +1555,262 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="64"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="46"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="64"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="46"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="67"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="54"/>
-      <c r="D8" s="54"/>
-      <c r="E8" s="54"/>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="54"/>
-      <c r="I8" s="55"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75"/>
+      <c r="H8" s="75"/>
+      <c r="I8" s="76"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="57"/>
-      <c r="G9" s="57"/>
-      <c r="H9" s="57"/>
-      <c r="I9" s="58"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="78"/>
+      <c r="G9" s="78"/>
+      <c r="H9" s="78"/>
+      <c r="I9" s="79"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="65" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="45"/>
-      <c r="D10" s="45"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="45" t="s">
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="67"/>
+      <c r="F10" s="66" t="s">
         <v>19</v>
       </c>
-      <c r="G10" s="45"/>
-      <c r="H10" s="45"/>
-      <c r="I10" s="46"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="67"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="50"/>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="51"/>
-      <c r="G11" s="51"/>
-      <c r="H11" s="51"/>
-      <c r="I11" s="52"/>
+      <c r="B11" s="71"/>
+      <c r="C11" s="72"/>
+      <c r="D11" s="72"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="72"/>
+      <c r="G11" s="72"/>
+      <c r="H11" s="72"/>
+      <c r="I11" s="73"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="44" t="s">
+      <c r="B12" s="65" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="45"/>
-      <c r="D12" s="45"/>
-      <c r="E12" s="45"/>
-      <c r="F12" s="45"/>
-      <c r="G12" s="45"/>
-      <c r="H12" s="45"/>
-      <c r="I12" s="46"/>
+      <c r="C12" s="66"/>
+      <c r="D12" s="66"/>
+      <c r="E12" s="66"/>
+      <c r="F12" s="66"/>
+      <c r="G12" s="66"/>
+      <c r="H12" s="66"/>
+      <c r="I12" s="67"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="52"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="73"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="41" t="s">
+      <c r="B14" s="62" t="s">
         <v>21</v>
       </c>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="43"/>
+      <c r="C14" s="63"/>
+      <c r="D14" s="63"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="63"/>
+      <c r="G14" s="63"/>
+      <c r="H14" s="63"/>
+      <c r="I14" s="64"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="50"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
-      <c r="G15" s="51"/>
-      <c r="H15" s="51"/>
-      <c r="I15" s="52"/>
-    </row>
-    <row r="16" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="20" t="s">
+      <c r="B15" s="71"/>
+      <c r="C15" s="72"/>
+      <c r="D15" s="72"/>
+      <c r="E15" s="72"/>
+      <c r="F15" s="72"/>
+      <c r="G15" s="72"/>
+      <c r="H15" s="72"/>
+      <c r="I15" s="73"/>
+    </row>
+    <row r="16" spans="2:9" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="22"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="42"/>
     </row>
     <row r="17" spans="2:9" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="59" t="s">
+      <c r="B17" s="62" t="s">
         <v>23</v>
       </c>
-      <c r="C17" s="60"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="60"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="60"/>
-      <c r="H17" s="60"/>
-      <c r="I17" s="61"/>
-    </row>
-    <row r="18" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B18" s="47" t="s">
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="63"/>
+      <c r="G17" s="63"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="64"/>
+    </row>
+    <row r="18" spans="2:9" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="80" t="s">
+        <v>49</v>
+      </c>
+      <c r="C18" s="81"/>
+      <c r="D18" s="81"/>
+      <c r="E18" s="81"/>
+      <c r="F18" s="81"/>
+      <c r="G18" s="81"/>
+      <c r="H18" s="81"/>
+      <c r="I18" s="82"/>
+    </row>
+    <row r="19" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="83"/>
+      <c r="C19" s="84"/>
+      <c r="D19" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="17" t="s">
+        <v>55</v>
+      </c>
+      <c r="F19" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="G19" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="I19" s="10"/>
+    </row>
+    <row r="20" spans="2:9" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="11"/>
+      <c r="C20" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="16"/>
+    </row>
+    <row r="21" spans="2:9" ht="21.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="12"/>
+      <c r="C21" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="16"/>
+    </row>
+    <row r="22" spans="2:9" ht="22.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="11"/>
+      <c r="C22" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="8"/>
+      <c r="E22" s="8"/>
+      <c r="F22" s="8"/>
+      <c r="G22" s="8"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="16"/>
+    </row>
+    <row r="23" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B23" s="13"/>
+      <c r="C23" s="14"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="15"/>
+    </row>
+    <row r="24" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B24" s="68" t="s">
         <v>12</v>
       </c>
-      <c r="C18" s="48"/>
-      <c r="D18" s="48"/>
-      <c r="E18" s="48"/>
-      <c r="F18" s="48"/>
-      <c r="G18" s="48"/>
-      <c r="H18" s="48"/>
-      <c r="I18" s="49"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="C22" s="2"/>
+      <c r="C24" s="69"/>
+      <c r="D24" s="69"/>
+      <c r="E24" s="69"/>
+      <c r="F24" s="69"/>
+      <c r="G24" s="69"/>
+      <c r="H24" s="69"/>
+      <c r="I24" s="70"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C28" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="14">
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="F2:I2"/>
     <mergeCell ref="B4:I5"/>
-    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B24:I24"/>
     <mergeCell ref="B14:I15"/>
     <mergeCell ref="B6:I7"/>
     <mergeCell ref="B8:I9"/>
@@ -1572,8 +1819,11 @@
     <mergeCell ref="B12:I13"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B17:I17"/>
+    <mergeCell ref="B18:I18"/>
+    <mergeCell ref="B19:C19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1581,131 +1831,131 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5244648D-77D7-46EA-93CC-F575EA20A8AE}">
   <dimension ref="B2:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+    <sheetView zoomScale="107" workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="23" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="43"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="64"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="44"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="46"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="67"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="62" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="43"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="64"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="46"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="67"/>
     </row>
     <row r="7" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B7" s="20" t="s">
+      <c r="B7" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="21"/>
-      <c r="D7" s="21"/>
-      <c r="E7" s="21"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
       <c r="F7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="66"/>
+      <c r="G7" s="94"/>
+      <c r="H7" s="94"/>
+      <c r="I7" s="95"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="62" t="s">
+      <c r="B8" s="91" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
-      <c r="H8" s="63"/>
-      <c r="I8" s="64"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="92"/>
+      <c r="F8" s="92"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="92"/>
+      <c r="I8" s="93"/>
     </row>
     <row r="9" spans="2:9" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="56"/>
-      <c r="C9" s="57"/>
-      <c r="D9" s="57"/>
-      <c r="E9" s="57"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
-      <c r="H9" s="63"/>
-      <c r="I9" s="64"/>
+      <c r="B9" s="77"/>
+      <c r="C9" s="78"/>
+      <c r="D9" s="78"/>
+      <c r="E9" s="78"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="92"/>
+      <c r="I9" s="93"/>
     </row>
     <row r="10" spans="2:9" ht="39" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="59" t="s">
+      <c r="B10" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="60"/>
-      <c r="D10" s="60"/>
-      <c r="E10" s="60"/>
-      <c r="F10" s="59" t="s">
+      <c r="C10" s="89"/>
+      <c r="D10" s="89"/>
+      <c r="E10" s="89"/>
+      <c r="F10" s="88" t="s">
         <v>29</v>
       </c>
-      <c r="G10" s="60"/>
-      <c r="H10" s="60"/>
-      <c r="I10" s="61"/>
+      <c r="G10" s="89"/>
+      <c r="H10" s="89"/>
+      <c r="I10" s="90"/>
     </row>
     <row r="11" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="47" t="s">
+      <c r="B11" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="C11" s="48"/>
-      <c r="D11" s="48"/>
-      <c r="E11" s="48"/>
-      <c r="F11" s="48"/>
-      <c r="G11" s="48"/>
-      <c r="H11" s="48"/>
-      <c r="I11" s="49"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="10">
@@ -1748,18 +1998,18 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="96" t="s">
         <v>30</v>
       </c>
-      <c r="C2" s="68"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="9" t="s">
+      <c r="C2" s="97"/>
+      <c r="D2" s="97"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="2:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="7" t="s">
@@ -1768,148 +2018,148 @@
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="76"/>
+      <c r="F3" s="68"/>
+      <c r="G3" s="69"/>
+      <c r="H3" s="69"/>
+      <c r="I3" s="70"/>
     </row>
     <row r="4" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="19"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="43"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="64"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-      <c r="H6" s="45"/>
-      <c r="I6" s="46"/>
+      <c r="B6" s="65"/>
+      <c r="C6" s="66"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="66"/>
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="66"/>
+      <c r="I6" s="67"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="42"/>
-      <c r="D7" s="42"/>
-      <c r="E7" s="42"/>
-      <c r="F7" s="42"/>
-      <c r="G7" s="42"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="43"/>
+      <c r="C7" s="63"/>
+      <c r="D7" s="63"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="63"/>
+      <c r="G7" s="63"/>
+      <c r="H7" s="63"/>
+      <c r="I7" s="64"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="44"/>
-      <c r="C8" s="45"/>
-      <c r="D8" s="45"/>
-      <c r="E8" s="45"/>
-      <c r="F8" s="45"/>
-      <c r="G8" s="45"/>
-      <c r="H8" s="45"/>
-      <c r="I8" s="46"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="66"/>
+      <c r="D8" s="66"/>
+      <c r="E8" s="66"/>
+      <c r="F8" s="66"/>
+      <c r="G8" s="66"/>
+      <c r="H8" s="66"/>
+      <c r="I8" s="67"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="53" t="s">
+      <c r="B9" s="74" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="54"/>
-      <c r="D9" s="54"/>
-      <c r="E9" s="54"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="54"/>
-      <c r="H9" s="54"/>
-      <c r="I9" s="55"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="76"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="56"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="58"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="79"/>
     </row>
     <row r="11" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="21"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="22"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="41"/>
+      <c r="G11" s="41"/>
+      <c r="H11" s="41"/>
+      <c r="I11" s="42"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="41" t="s">
+      <c r="B12" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="42" t="s">
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="42"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="43"/>
+      <c r="G12" s="63"/>
+      <c r="H12" s="63"/>
+      <c r="I12" s="64"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="50"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="52"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="52"/>
+      <c r="B13" s="71"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="73"/>
     </row>
     <row r="14" spans="2:9" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="70" t="s">
+      <c r="B14" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="71"/>
-      <c r="D14" s="71"/>
-      <c r="E14" s="71"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="72"/>
-      <c r="H14" s="72"/>
-      <c r="I14" s="73"/>
+      <c r="C14" s="100"/>
+      <c r="D14" s="100"/>
+      <c r="E14" s="100"/>
+      <c r="F14" s="101"/>
+      <c r="G14" s="101"/>
+      <c r="H14" s="101"/>
+      <c r="I14" s="102"/>
     </row>
     <row r="15" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B15" s="47" t="s">
+      <c r="B15" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="48"/>
-      <c r="D15" s="48"/>
-      <c r="E15" s="48"/>
-      <c r="F15" s="48"/>
-      <c r="G15" s="48"/>
-      <c r="H15" s="48"/>
-      <c r="I15" s="49"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -1941,178 +2191,178 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="42"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="64"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="46"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="64"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="46"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="67"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="43"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="64"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="50"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-      <c r="G9" s="51"/>
-      <c r="H9" s="51"/>
-      <c r="I9" s="52"/>
+      <c r="B9" s="71"/>
+      <c r="C9" s="72"/>
+      <c r="D9" s="72"/>
+      <c r="E9" s="72"/>
+      <c r="F9" s="72"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="72"/>
+      <c r="I9" s="73"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="62" t="s">
+      <c r="B10" s="91" t="s">
         <v>40</v>
       </c>
-      <c r="C10" s="63"/>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
-      <c r="H10" s="63"/>
-      <c r="I10" s="64"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="92"/>
+      <c r="G10" s="92"/>
+      <c r="H10" s="92"/>
+      <c r="I10" s="93"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="56"/>
-      <c r="C11" s="57"/>
-      <c r="D11" s="57"/>
-      <c r="E11" s="57"/>
-      <c r="F11" s="57"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="57"/>
-      <c r="I11" s="58"/>
+      <c r="B11" s="77"/>
+      <c r="C11" s="78"/>
+      <c r="D11" s="78"/>
+      <c r="E11" s="78"/>
+      <c r="F11" s="78"/>
+      <c r="G11" s="78"/>
+      <c r="H11" s="78"/>
+      <c r="I11" s="79"/>
     </row>
     <row r="12" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="12"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="21"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="22"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="41"/>
+      <c r="H12" s="41"/>
+      <c r="I12" s="42"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="41" t="s">
+      <c r="B13" s="62" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="43"/>
-      <c r="F13" s="42" t="s">
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="G13" s="42"/>
-      <c r="H13" s="42"/>
-      <c r="I13" s="43"/>
+      <c r="G13" s="63"/>
+      <c r="H13" s="63"/>
+      <c r="I13" s="64"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="50"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="51"/>
-      <c r="G14" s="51"/>
-      <c r="H14" s="51"/>
-      <c r="I14" s="52"/>
+      <c r="B14" s="71"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="72"/>
+      <c r="H14" s="72"/>
+      <c r="I14" s="73"/>
     </row>
     <row r="15" spans="2:9" ht="64.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="77" t="s">
+      <c r="B15" s="103" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="78"/>
-      <c r="D15" s="78"/>
-      <c r="E15" s="78"/>
-      <c r="F15" s="79"/>
-      <c r="G15" s="79"/>
-      <c r="H15" s="79"/>
-      <c r="I15" s="80"/>
+      <c r="C15" s="104"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="104"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="105"/>
+      <c r="H15" s="105"/>
+      <c r="I15" s="106"/>
     </row>
     <row r="16" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B16" s="47" t="s">
+      <c r="B16" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="48"/>
-      <c r="D16" s="48"/>
-      <c r="E16" s="48"/>
-      <c r="F16" s="48"/>
-      <c r="G16" s="48"/>
-      <c r="H16" s="48"/>
-      <c r="I16" s="49"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2150,188 +2400,188 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="40" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="21"/>
-      <c r="D3" s="21"/>
-      <c r="E3" s="21"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="21"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="22"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
+      <c r="G3" s="41"/>
+      <c r="H3" s="41"/>
+      <c r="I3" s="42"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="64"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="46"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="64"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="46"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="67"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="42"/>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
-      <c r="G8" s="42"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="43"/>
+      <c r="C8" s="63"/>
+      <c r="D8" s="63"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="63"/>
+      <c r="G8" s="63"/>
+      <c r="H8" s="63"/>
+      <c r="I8" s="64"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="44"/>
-      <c r="C9" s="45"/>
-      <c r="D9" s="45"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="45"/>
-      <c r="I9" s="46"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="66"/>
+      <c r="D9" s="66"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
+      <c r="G9" s="66"/>
+      <c r="H9" s="66"/>
+      <c r="I9" s="67"/>
     </row>
     <row r="10" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B10" s="81" t="s">
+      <c r="B10" s="107" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="82"/>
-      <c r="D10" s="82"/>
-      <c r="E10" s="82"/>
-      <c r="F10" s="82"/>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="83"/>
+      <c r="C10" s="108"/>
+      <c r="D10" s="108"/>
+      <c r="E10" s="108"/>
+      <c r="F10" s="108"/>
+      <c r="G10" s="108"/>
+      <c r="H10" s="108"/>
+      <c r="I10" s="109"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="85"/>
-      <c r="D11" s="86"/>
-      <c r="E11" s="84" t="s">
+      <c r="C11" s="111"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="110" t="s">
         <v>46</v>
       </c>
-      <c r="F11" s="85"/>
-      <c r="G11" s="86"/>
-      <c r="H11" s="84" t="s">
+      <c r="F11" s="111"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="86"/>
+      <c r="I11" s="112"/>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B12" s="87"/>
-      <c r="C12" s="88"/>
-      <c r="D12" s="89"/>
-      <c r="E12" s="87"/>
-      <c r="F12" s="88"/>
-      <c r="G12" s="89"/>
-      <c r="H12" s="87"/>
-      <c r="I12" s="89"/>
+      <c r="B12" s="113"/>
+      <c r="C12" s="114"/>
+      <c r="D12" s="115"/>
+      <c r="E12" s="113"/>
+      <c r="F12" s="114"/>
+      <c r="G12" s="115"/>
+      <c r="H12" s="113"/>
+      <c r="I12" s="115"/>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B13" s="87"/>
-      <c r="C13" s="88"/>
-      <c r="D13" s="89"/>
-      <c r="E13" s="87"/>
-      <c r="F13" s="88"/>
-      <c r="G13" s="89"/>
-      <c r="H13" s="87"/>
-      <c r="I13" s="89"/>
+      <c r="B13" s="113"/>
+      <c r="C13" s="114"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="113"/>
+      <c r="F13" s="114"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="113"/>
+      <c r="I13" s="115"/>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B14" s="87"/>
-      <c r="C14" s="88"/>
-      <c r="D14" s="89"/>
-      <c r="E14" s="87"/>
-      <c r="F14" s="88"/>
-      <c r="G14" s="89"/>
-      <c r="H14" s="87"/>
-      <c r="I14" s="89"/>
+      <c r="B14" s="113"/>
+      <c r="C14" s="114"/>
+      <c r="D14" s="115"/>
+      <c r="E14" s="113"/>
+      <c r="F14" s="114"/>
+      <c r="G14" s="115"/>
+      <c r="H14" s="113"/>
+      <c r="I14" s="115"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B15" s="90"/>
-      <c r="C15" s="91"/>
-      <c r="D15" s="92"/>
-      <c r="E15" s="90"/>
-      <c r="F15" s="91"/>
-      <c r="G15" s="92"/>
-      <c r="H15" s="90"/>
-      <c r="I15" s="92"/>
+      <c r="B15" s="116"/>
+      <c r="C15" s="117"/>
+      <c r="D15" s="118"/>
+      <c r="E15" s="116"/>
+      <c r="F15" s="117"/>
+      <c r="G15" s="118"/>
+      <c r="H15" s="116"/>
+      <c r="I15" s="118"/>
     </row>
     <row r="16" spans="2:9" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="50" t="s">
+      <c r="B16" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
-      <c r="G16" s="51"/>
-      <c r="H16" s="51"/>
-      <c r="I16" s="52"/>
+      <c r="C16" s="72"/>
+      <c r="D16" s="72"/>
+      <c r="E16" s="72"/>
+      <c r="F16" s="72"/>
+      <c r="G16" s="72"/>
+      <c r="H16" s="72"/>
+      <c r="I16" s="73"/>
     </row>
     <row r="17" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B17" s="47" t="s">
+      <c r="B17" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="C17" s="48"/>
-      <c r="D17" s="48"/>
-      <c r="E17" s="48"/>
-      <c r="F17" s="48"/>
-      <c r="G17" s="48"/>
-      <c r="H17" s="48"/>
-      <c r="I17" s="49"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2363,158 +2613,158 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="23" t="s">
         <v>48</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="93" t="s">
+      <c r="B3" s="119" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="94"/>
-      <c r="E3" s="94"/>
-      <c r="F3" s="94"/>
-      <c r="G3" s="94"/>
-      <c r="H3" s="94"/>
-      <c r="I3" s="95"/>
+      <c r="C3" s="120"/>
+      <c r="D3" s="120"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="120"/>
+      <c r="G3" s="120"/>
+      <c r="H3" s="120"/>
+      <c r="I3" s="121"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="65" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="46"/>
+      <c r="C4" s="66"/>
+      <c r="D4" s="66"/>
+      <c r="E4" s="66"/>
+      <c r="F4" s="66"/>
+      <c r="G4" s="66"/>
+      <c r="H4" s="66"/>
+      <c r="I4" s="67"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B5" s="50"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="51"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="52"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="72"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
+      <c r="G5" s="72"/>
+      <c r="H5" s="72"/>
+      <c r="I5" s="73"/>
     </row>
     <row r="6" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="122" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="97"/>
-      <c r="D6" s="97"/>
-      <c r="E6" s="97"/>
-      <c r="F6" s="97"/>
-      <c r="G6" s="97"/>
-      <c r="H6" s="97"/>
-      <c r="I6" s="98"/>
+      <c r="C6" s="123"/>
+      <c r="D6" s="123"/>
+      <c r="E6" s="123"/>
+      <c r="F6" s="123"/>
+      <c r="G6" s="123"/>
+      <c r="H6" s="123"/>
+      <c r="I6" s="124"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B7" s="84" t="s">
+      <c r="B7" s="110" t="s">
         <v>45</v>
       </c>
-      <c r="C7" s="85"/>
-      <c r="D7" s="86"/>
-      <c r="E7" s="84" t="s">
+      <c r="C7" s="111"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="110" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="85"/>
-      <c r="G7" s="86"/>
-      <c r="H7" s="84" t="s">
+      <c r="F7" s="111"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="110" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="86"/>
+      <c r="I7" s="112"/>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B8" s="87"/>
-      <c r="C8" s="88"/>
-      <c r="D8" s="89"/>
-      <c r="E8" s="87"/>
-      <c r="F8" s="88"/>
-      <c r="G8" s="89"/>
-      <c r="H8" s="87"/>
-      <c r="I8" s="89"/>
+      <c r="B8" s="113"/>
+      <c r="C8" s="114"/>
+      <c r="D8" s="115"/>
+      <c r="E8" s="113"/>
+      <c r="F8" s="114"/>
+      <c r="G8" s="115"/>
+      <c r="H8" s="113"/>
+      <c r="I8" s="115"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B9" s="87"/>
-      <c r="C9" s="88"/>
-      <c r="D9" s="89"/>
-      <c r="E9" s="87"/>
-      <c r="F9" s="88"/>
-      <c r="G9" s="89"/>
-      <c r="H9" s="87"/>
-      <c r="I9" s="89"/>
+      <c r="B9" s="113"/>
+      <c r="C9" s="114"/>
+      <c r="D9" s="115"/>
+      <c r="E9" s="113"/>
+      <c r="F9" s="114"/>
+      <c r="G9" s="115"/>
+      <c r="H9" s="113"/>
+      <c r="I9" s="115"/>
     </row>
     <row r="10" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B10" s="87"/>
-      <c r="C10" s="88"/>
-      <c r="D10" s="89"/>
-      <c r="E10" s="87"/>
-      <c r="F10" s="88"/>
-      <c r="G10" s="89"/>
-      <c r="H10" s="87"/>
-      <c r="I10" s="89"/>
+      <c r="B10" s="113"/>
+      <c r="C10" s="114"/>
+      <c r="D10" s="115"/>
+      <c r="E10" s="113"/>
+      <c r="F10" s="114"/>
+      <c r="G10" s="115"/>
+      <c r="H10" s="113"/>
+      <c r="I10" s="115"/>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B11" s="90"/>
-      <c r="C11" s="91"/>
-      <c r="D11" s="92"/>
-      <c r="E11" s="90"/>
-      <c r="F11" s="91"/>
-      <c r="G11" s="92"/>
-      <c r="H11" s="90"/>
-      <c r="I11" s="92"/>
+      <c r="B11" s="116"/>
+      <c r="C11" s="117"/>
+      <c r="D11" s="118"/>
+      <c r="E11" s="116"/>
+      <c r="F11" s="117"/>
+      <c r="G11" s="118"/>
+      <c r="H11" s="116"/>
+      <c r="I11" s="118"/>
     </row>
     <row r="12" spans="2:9" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="77" t="s">
         <v>41</v>
       </c>
-      <c r="C12" s="57"/>
-      <c r="D12" s="57"/>
-      <c r="E12" s="58"/>
-      <c r="F12" s="57" t="s">
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="79"/>
+      <c r="F12" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="57"/>
-      <c r="H12" s="57"/>
-      <c r="I12" s="58"/>
-    </row>
-    <row r="13" spans="2:9" ht="55.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="50" t="s">
+      <c r="G12" s="78"/>
+      <c r="H12" s="78"/>
+      <c r="I12" s="79"/>
+    </row>
+    <row r="13" spans="2:9" ht="55.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B13" s="71" t="s">
         <v>35</v>
       </c>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
-      <c r="G13" s="51"/>
-      <c r="H13" s="51"/>
-      <c r="I13" s="52"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="72"/>
+      <c r="H13" s="72"/>
+      <c r="I13" s="73"/>
     </row>
     <row r="14" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B14" s="47" t="s">
+      <c r="B14" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="48"/>
-      <c r="D14" s="48"/>
-      <c r="E14" s="48"/>
-      <c r="F14" s="48"/>
-      <c r="G14" s="48"/>
-      <c r="H14" s="48"/>
-      <c r="I14" s="49"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="12">
@@ -2546,18 +2796,18 @@
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="2" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="8" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="24"/>
+      <c r="E2" s="24"/>
+      <c r="F2" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="61"/>
     </row>
     <row r="3" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B3" s="3" t="s">
@@ -2572,72 +2822,72 @@
       <c r="I3" s="5"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="62" t="s">
         <v>9</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="43"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="64"/>
     </row>
     <row r="5" spans="2:9" ht="53.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="45"/>
-      <c r="I5" s="46"/>
+      <c r="B5" s="65"/>
+      <c r="C5" s="66"/>
+      <c r="D5" s="66"/>
+      <c r="E5" s="66"/>
+      <c r="F5" s="66"/>
+      <c r="G5" s="66"/>
+      <c r="H5" s="66"/>
+      <c r="I5" s="67"/>
     </row>
     <row r="6" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="41" t="s">
+      <c r="B6" s="62" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="43"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="64"/>
     </row>
     <row r="7" spans="2:9" ht="32.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="50"/>
-      <c r="C7" s="51"/>
-      <c r="D7" s="51"/>
-      <c r="E7" s="51"/>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="52"/>
+      <c r="B7" s="71"/>
+      <c r="C7" s="72"/>
+      <c r="D7" s="72"/>
+      <c r="E7" s="72"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="72"/>
+      <c r="H7" s="72"/>
+      <c r="I7" s="73"/>
     </row>
     <row r="8" spans="2:9" ht="56.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="99" t="s">
         <v>35</v>
       </c>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="72"/>
-      <c r="G8" s="72"/>
-      <c r="H8" s="72"/>
-      <c r="I8" s="73"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="100"/>
+      <c r="E8" s="100"/>
+      <c r="F8" s="101"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+      <c r="I8" s="102"/>
     </row>
     <row r="9" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B9" s="47" t="s">
+      <c r="B9" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="49"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="87"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>